<commit_message>
- Laatste verwijzingen naar HODOR verwijderd - Demo access database's toegevoegd (moet nog verder uitgebreid worden) - Laatste vergelijkingen van SWF toegevoegd
</commit_message>
<xml_diff>
--- a/data/HODOR_CHECK.xlsx
+++ b/data/HODOR_CHECK.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduard\ownCloud\ontwikkelen\github.com\GegevensVergelijker.metwijzigingen\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="HODOR_CHECK" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
   <si>
     <t>CHECKNAME</t>
   </si>
@@ -82,6 +87,18 @@
     <t>bagobjectid</t>
   </si>
   <si>
+    <t>LITTENS_ISPIEGEL_K</t>
+  </si>
+  <si>
+    <t>K_LITTENS</t>
+  </si>
+  <si>
+    <t>LITTENS_ISPIEGEL_L</t>
+  </si>
+  <si>
+    <t>L_LITTENS</t>
+  </si>
+  <si>
     <t>DDS_VOA_ALLEEN_AANTEKENING</t>
   </si>
   <si>
@@ -110,6 +127,18 @@
   </si>
   <si>
     <t>GOED_VBO_VBO_NR</t>
+  </si>
+  <si>
+    <t>HARL_ISPIEGEL_K</t>
+  </si>
+  <si>
+    <t>K_HARLINGEN</t>
+  </si>
+  <si>
+    <t>HARL_ISPIEGEL_L</t>
+  </si>
+  <si>
+    <t>L_HARLINGEN</t>
   </si>
   <si>
     <t>DDS_VOA_GEEN_AANTEKENING</t>
@@ -194,8 +223,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:F9" totalsRowShown="0">
-  <autoFilter ref="A1:F9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel2" displayName="Tabel2" ref="A1:F13" totalsRowShown="0">
+  <autoFilter ref="A1:F13"/>
   <tableColumns count="6">
     <tableColumn id="1" name="CHECKNAME"/>
     <tableColumn id="2" name="DATASOURCENAME"/>
@@ -225,7 +254,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -237,7 +266,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -505,20 +534,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -626,16 +658,16 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F6" s="1">
         <v>-1</v>
@@ -643,19 +675,19 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F7" s="1">
         <v>-1</v>
@@ -663,19 +695,19 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
         <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>25</v>
       </c>
       <c r="F8" s="1">
         <v>-1</v>
@@ -683,29 +715,108 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F9" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="1">
         <v>-1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>